<commit_message>
Implemented LeapProvider (converting, ...)
</commit_message>
<xml_diff>
--- a/doc/timelog/p.xlsx
+++ b/doc/timelog/p.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="7020" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Domänenmodell</t>
+  </si>
+  <si>
+    <t>LeapProvider + Convert (untested), Contracts unfinished</t>
   </si>
 </sst>
 </file>
@@ -501,12 +504,21 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="2">
+        <v>41790</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,7 +740,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31" s="3">
         <f>SUM(D2:D30)</f>
-        <v>0.29166666666666674</v>
+        <v>0.41666666666666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Added Visualizer  * Added SharpDX.WPF
</commit_message>
<xml_diff>
--- a/doc/timelog/p.xlsx
+++ b/doc/timelog/p.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="8715" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>LeapProvider + Convert (untested), Contracts unfinished</t>
+  </si>
+  <si>
+    <t>SharpDX recherchen, SharpDX.WPF einbinden</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,12 +525,21 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="2">
+        <v>41790</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.8125</v>
+      </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,7 +752,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31" s="3">
         <f>SUM(D2:D30)</f>
-        <v>0.41666666666666674</v>
+        <v>0.47916666666666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>